<commit_message>
current file as per website iteration 1
</commit_message>
<xml_diff>
--- a/Groups in Community Connect.xlsx
+++ b/Groups in Community Connect.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/souravroychoudhury/Desktop/SocialMedia 13/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/souravroychoudhury/Desktop/testing_deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D049820D-4475-A947-BE12-21E4C984C142}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B0A394-438B-5D4C-84DB-2FF0619988B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="580" windowWidth="22720" windowHeight="10520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1540" yWindow="1460" windowWidth="22720" windowHeight="10520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
   <si>
     <t>User ID</t>
   </si>
@@ -37,73 +37,172 @@
     <t>Gender</t>
   </si>
   <si>
-    <t>Khyati</t>
-  </si>
-  <si>
     <t>Blue, Red</t>
   </si>
   <si>
-    <t>Sourav</t>
-  </si>
-  <si>
     <t>Blue</t>
   </si>
   <si>
-    <t>Nana</t>
-  </si>
-  <si>
     <t>Red</t>
   </si>
   <si>
-    <t>Iris</t>
-  </si>
-  <si>
-    <t>Josh</t>
-  </si>
-  <si>
     <t>user_id</t>
   </si>
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>Abagail</t>
-  </si>
-  <si>
-    <t>km_062020</t>
-  </si>
-  <si>
-    <t>so_062020</t>
-  </si>
-  <si>
-    <t>aba_062020</t>
-  </si>
-  <si>
-    <t>na_062020</t>
-  </si>
-  <si>
-    <t>ir_062020</t>
-  </si>
-  <si>
-    <t>jo_062020</t>
+    <t>Samira Shaikh</t>
+  </si>
+  <si>
+    <t>sroychou@uncc.edu</t>
+  </si>
+  <si>
+    <t>samirashaikh@uncc.edu</t>
   </si>
   <si>
     <t>kmahaja2@uncc.edu</t>
   </si>
   <si>
-    <t>sroychou@uncc.edu</t>
+    <t>slevens@uncc.edu</t>
+  </si>
+  <si>
+    <t>acart108@uncc.edu</t>
+  </si>
+  <si>
+    <t>edoe1@uncc.edu</t>
+  </si>
+  <si>
+    <t>vflahert@uncc.edu</t>
+  </si>
+  <si>
+    <t>kmchouel@uncc.edu</t>
+  </si>
+  <si>
+    <t>aphrakou@uncc.edu</t>
+  </si>
+  <si>
+    <t>eshaffe2@uncc.edu</t>
+  </si>
+  <si>
+    <t>vwheele1@uncc.edu</t>
   </si>
   <si>
     <t>ahiggi27@uncc.edu</t>
   </si>
   <si>
+    <t>Sara Levens</t>
+  </si>
+  <si>
+    <t>jgordo42@uncc.edu</t>
+  </si>
+  <si>
+    <t>ihudson@uncc.edu</t>
+  </si>
+  <si>
     <t>nsledzie@uncc.edu</t>
   </si>
   <si>
-    <t>ihudson@uncc.edu</t>
-  </si>
-  <si>
-    <t>jgordo42@uncc.edu</t>
+    <t>April Phrakousonh</t>
+  </si>
+  <si>
+    <t>Edward Shaffer</t>
+  </si>
+  <si>
+    <t>Victoria Wheeler</t>
+  </si>
+  <si>
+    <t>Josh Gordon</t>
+  </si>
+  <si>
+    <t>Iris Hudson</t>
+  </si>
+  <si>
+    <t>Nana Sledzieski</t>
+  </si>
+  <si>
+    <t>Olivia Lawless</t>
+  </si>
+  <si>
+    <t>Katelyn Mchouell</t>
+  </si>
+  <si>
+    <t>Victoria Flaherty</t>
+  </si>
+  <si>
+    <t>Elikem Doe</t>
+  </si>
+  <si>
+    <t>Antwan Carter</t>
+  </si>
+  <si>
+    <t>Abagail Higgins</t>
+  </si>
+  <si>
+    <t>Sourav Roy Choudhury</t>
+  </si>
+  <si>
+    <t>Khyati Mahajan</t>
+  </si>
+  <si>
+    <t>km_07_2020</t>
+  </si>
+  <si>
+    <t>so_07_2020</t>
+  </si>
+  <si>
+    <t>ah_07_2020</t>
+  </si>
+  <si>
+    <t>sl_07_2020</t>
+  </si>
+  <si>
+    <t>ac_07_2020</t>
+  </si>
+  <si>
+    <t>ed_07_2020</t>
+  </si>
+  <si>
+    <t>vf_07_2020</t>
+  </si>
+  <si>
+    <t>kc_07_2020</t>
+  </si>
+  <si>
+    <t>ap_07_2020</t>
+  </si>
+  <si>
+    <t>es_07_2020</t>
+  </si>
+  <si>
+    <t>vw_07_2020</t>
+  </si>
+  <si>
+    <t>jg_07_2020</t>
+  </si>
+  <si>
+    <t>ih_07_2020</t>
+  </si>
+  <si>
+    <t>ns_07_2020</t>
+  </si>
+  <si>
+    <t>ol_07_2020</t>
+  </si>
+  <si>
+    <t>ss_07_2020</t>
+  </si>
+  <si>
+    <t>olawless@uncc.edu</t>
+  </si>
+  <si>
+    <t>sjohn357@uncc.edu</t>
+  </si>
+  <si>
+    <t>Samantha Johnson</t>
+  </si>
+  <si>
+    <t>sj_07_2020</t>
   </si>
 </sst>
 </file>
@@ -120,16 +219,19 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -377,16 +479,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -397,10 +499,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -414,92 +516,261 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>19</v>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>8</v>
+      <c r="E13" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{D5AF0C67-499E-6543-96AA-EF9C900C0B62}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{51B00B10-E5C4-4141-B096-A4DE23C76CAD}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{AB41F2D0-0032-394A-A4B9-1C385DCB05DF}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{5C2DB905-6C7F-3B40-A3BA-620D9B8F51B2}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{662817E4-C378-3740-B872-0E38C51F9ABC}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{F046659C-85D1-E149-A5FC-873E68E8D97B}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{3585F3CF-7638-D140-B7AA-C54367CDB840}"/>
+    <hyperlink ref="D9" r:id="rId6" xr:uid="{A72CF78B-53EA-B344-91B3-F4B480D233F5}"/>
+    <hyperlink ref="D10" r:id="rId7" xr:uid="{E056041F-F28F-A64D-8103-17E1E167A624}"/>
+    <hyperlink ref="D11" r:id="rId8" xr:uid="{2EA757E7-9BE9-5B47-9DED-56A713203E3D}"/>
+    <hyperlink ref="D12" r:id="rId9" xr:uid="{94CB5BE4-09E2-2040-9A4D-56018EDBDC8C}"/>
+    <hyperlink ref="D13" r:id="rId10" xr:uid="{AE00EEF4-E421-6E45-94FB-0A922552D82B}"/>
+    <hyperlink ref="D4" r:id="rId11" display="mailto:ahiggi27@uncc.edu" xr:uid="{481817AF-6DAC-0D47-99AC-8B22AF2939FD}"/>
+    <hyperlink ref="D14" r:id="rId12" xr:uid="{3129B820-ADBE-0642-89FD-5423BF219216}"/>
+    <hyperlink ref="D15" r:id="rId13" xr:uid="{79FF13ED-EB6F-4F4D-BD52-E60C115E54EE}"/>
+    <hyperlink ref="D16" r:id="rId14" xr:uid="{467A5FDB-D7E4-E648-A15C-AE066C7B0A2B}"/>
+    <hyperlink ref="D17" r:id="rId15" xr:uid="{F6FAE1A0-7E01-474A-B498-9E14F028070A}"/>
+    <hyperlink ref="D5" r:id="rId16" xr:uid="{E9ED72E5-CC8F-934A-BEBB-8C488148898C}"/>
+    <hyperlink ref="D18" r:id="rId17" display="mailto:sjohn357@uncc.edu" xr:uid="{7C8CF40B-E030-DD49-B6BC-1E5827909B00}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>